<commit_message>
all processed through 2019-05-27
</commit_message>
<xml_diff>
--- a/templates/Limno_GCrunfileTemplate_DONOTSAVE.xlsx
+++ b/templates/Limno_GCrunfileTemplate_DONOTSAVE.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brittnibertolet/OneDrive - nd.edu/underc-field-2019/data/gc2019underc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brittnibertolet/OneDrive - nd.edu/underc-field-2019/dataLogs/gc2019underc/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="11_1C0481BE3CDD15577FD25C06219C096B704D1EE5" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{B95B24C5-A291-704F-8FA9-ADD9BE70DDC6}"/>
+  <xr:revisionPtr revIDLastSave="183" documentId="11_1C0481BE3CDD15577FD25C06219C096B704D1EE5" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{94D36AA4-FA76-C542-83E4-3F685FEA94B0}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="23880" windowHeight="14580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="43">
   <si>
     <t>projectID</t>
   </si>
@@ -107,21 +107,9 @@
     <t>gc180508</t>
   </si>
   <si>
-    <t>runYYMMDDRR</t>
-  </si>
-  <si>
-    <t>YYMMDDRR</t>
-  </si>
-  <si>
     <t>Outlet</t>
   </si>
   <si>
-    <t>CR</t>
-  </si>
-  <si>
-    <t>HB</t>
-  </si>
-  <si>
     <t>standard034</t>
   </si>
   <si>
@@ -143,15 +131,6 @@
     <t>PA</t>
   </si>
   <si>
-    <t>Littoral1</t>
-  </si>
-  <si>
-    <t>Littoral2</t>
-  </si>
-  <si>
-    <t>Littoral3</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -159,6 +138,24 @@
   </si>
   <si>
     <t>lab</t>
+  </si>
+  <si>
+    <t>run19052301</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>algal</t>
+  </si>
+  <si>
+    <t>BES</t>
+  </si>
+  <si>
+    <t>algalBES</t>
   </si>
 </sst>
 </file>
@@ -501,13 +498,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -672,7 +669,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -680,7 +677,6 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1069,10 +1065,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R57"/>
+  <dimension ref="A1:R59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="113" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33:F43"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="75" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1163,10 +1159,10 @@
         <v>16</v>
       </c>
       <c r="D2" s="2">
-        <v>43605</v>
+        <v>43609</v>
       </c>
       <c r="E2" s="3">
-        <v>43605</v>
+        <v>43608</v>
       </c>
       <c r="F2" t="s">
         <v>16</v>
@@ -1181,13 +1177,13 @@
         <v>17</v>
       </c>
       <c r="J2" s="3">
-        <v>36526</v>
+        <v>43608</v>
       </c>
       <c r="K2" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="L2" s="2">
-        <v>36526</v>
+        <v>43608</v>
       </c>
       <c r="M2" s="1">
         <v>1</v>
@@ -1198,12 +1194,12 @@
       <c r="O2">
         <v>1</v>
       </c>
-      <c r="P2" t="s">
-        <v>27</v>
+      <c r="P2">
+        <v>19052301</v>
       </c>
       <c r="Q2" t="str">
         <f>CONCATENATE(O2,"_",P2)</f>
-        <v>1_YYMMDDRR</v>
+        <v>1_19052301</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
@@ -1217,7 +1213,10 @@
         <v>16</v>
       </c>
       <c r="D3" s="2">
-        <v>43605</v>
+        <v>43609</v>
+      </c>
+      <c r="E3" s="3">
+        <v>43608</v>
       </c>
       <c r="F3" t="s">
         <v>16</v>
@@ -1229,9 +1228,17 @@
         <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="J3" s="3">
+        <v>43608</v>
+      </c>
+      <c r="K3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="2">
+        <v>43608</v>
+      </c>
       <c r="M3" s="1">
         <v>1</v>
       </c>
@@ -1241,9 +1248,12 @@
       <c r="O3">
         <v>2</v>
       </c>
+      <c r="P3">
+        <v>19052301</v>
+      </c>
       <c r="Q3" t="str">
-        <f t="shared" ref="Q3:Q8" si="0">CONCATENATE(O3,"_",P3)</f>
-        <v>2_</v>
+        <f>CONCATENATE(O3,"_",P3)</f>
+        <v>2_19052301</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
@@ -1257,7 +1267,10 @@
         <v>16</v>
       </c>
       <c r="D4" s="2">
-        <v>43605</v>
+        <v>43609</v>
+      </c>
+      <c r="E4" s="3">
+        <v>43608</v>
       </c>
       <c r="F4" t="s">
         <v>16</v>
@@ -1269,9 +1282,17 @@
         <v>16</v>
       </c>
       <c r="I4" t="s">
-        <v>32</v>
-      </c>
-      <c r="L4" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="J4" s="3">
+        <v>43608</v>
+      </c>
+      <c r="K4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" s="2">
+        <v>43608</v>
+      </c>
       <c r="M4" s="1">
         <v>1</v>
       </c>
@@ -1281,9 +1302,12 @@
       <c r="O4">
         <v>3</v>
       </c>
+      <c r="P4">
+        <v>19052301</v>
+      </c>
       <c r="Q4" t="str">
-        <f t="shared" si="0"/>
-        <v>3_</v>
+        <f>CONCATENATE(O4,"_",P4)</f>
+        <v>3_19052301</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
@@ -1297,7 +1321,10 @@
         <v>16</v>
       </c>
       <c r="D5" s="2">
-        <v>43605</v>
+        <v>43609</v>
+      </c>
+      <c r="E5" s="3">
+        <v>43608</v>
       </c>
       <c r="F5" t="s">
         <v>16</v>
@@ -1309,9 +1336,17 @@
         <v>16</v>
       </c>
       <c r="I5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L5" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="J5" s="3">
+        <v>43608</v>
+      </c>
+      <c r="K5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="2">
+        <v>43608</v>
+      </c>
       <c r="M5" s="1">
         <v>1</v>
       </c>
@@ -1321,9 +1356,12 @@
       <c r="O5">
         <v>4</v>
       </c>
+      <c r="P5">
+        <v>19052301</v>
+      </c>
       <c r="Q5" t="str">
-        <f t="shared" si="0"/>
-        <v>4_</v>
+        <f t="shared" ref="Q5:Q17" si="0">CONCATENATE(O5,"_",P5)</f>
+        <v>4_19052301</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
@@ -1337,7 +1375,10 @@
         <v>16</v>
       </c>
       <c r="D6" s="2">
-        <v>43605</v>
+        <v>43609</v>
+      </c>
+      <c r="E6" s="3">
+        <v>43608</v>
       </c>
       <c r="F6" t="s">
         <v>16</v>
@@ -1349,9 +1390,17 @@
         <v>16</v>
       </c>
       <c r="I6" t="s">
-        <v>34</v>
-      </c>
-      <c r="L6" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="J6" s="3">
+        <v>43608</v>
+      </c>
+      <c r="K6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" s="2">
+        <v>43608</v>
+      </c>
       <c r="M6" s="1">
         <v>1</v>
       </c>
@@ -1361,9 +1410,12 @@
       <c r="O6">
         <v>5</v>
       </c>
+      <c r="P6">
+        <v>19052301</v>
+      </c>
       <c r="Q6" t="str">
         <f t="shared" si="0"/>
-        <v>5_</v>
+        <v>5_19052301</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
@@ -1377,7 +1429,10 @@
         <v>16</v>
       </c>
       <c r="D7" s="2">
-        <v>43605</v>
+        <v>43609</v>
+      </c>
+      <c r="E7" s="3">
+        <v>43608</v>
       </c>
       <c r="F7" t="s">
         <v>16</v>
@@ -1389,9 +1444,17 @@
         <v>16</v>
       </c>
       <c r="I7" t="s">
-        <v>35</v>
-      </c>
-      <c r="L7" s="2"/>
+        <v>31</v>
+      </c>
+      <c r="J7" s="3">
+        <v>43608</v>
+      </c>
+      <c r="K7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L7" s="2">
+        <v>43608</v>
+      </c>
       <c r="M7" s="1">
         <v>1</v>
       </c>
@@ -1401,9 +1464,12 @@
       <c r="O7">
         <v>6</v>
       </c>
+      <c r="P7">
+        <v>19052301</v>
+      </c>
       <c r="Q7" t="str">
         <f t="shared" si="0"/>
-        <v>6_</v>
+        <v>6_19052301</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -1417,7 +1483,10 @@
         <v>16</v>
       </c>
       <c r="D8" s="2">
-        <v>43605</v>
+        <v>43609</v>
+      </c>
+      <c r="E8" s="3">
+        <v>43608</v>
       </c>
       <c r="F8" t="s">
         <v>16</v>
@@ -1431,7 +1500,15 @@
       <c r="I8" t="s">
         <v>17</v>
       </c>
-      <c r="L8" s="2"/>
+      <c r="J8" s="3">
+        <v>43608</v>
+      </c>
+      <c r="K8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L8" s="2">
+        <v>43608</v>
+      </c>
       <c r="M8" s="1">
         <v>2</v>
       </c>
@@ -1441,9 +1518,12 @@
       <c r="O8">
         <v>7</v>
       </c>
+      <c r="P8">
+        <v>19052301</v>
+      </c>
       <c r="Q8" t="str">
         <f t="shared" si="0"/>
-        <v>7_</v>
+        <v>7_19052301</v>
       </c>
     </row>
     <row r="9" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1451,15 +1531,15 @@
         <v>15</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D9" s="2">
-        <v>43605</v>
-      </c>
-      <c r="E9" s="8"/>
+        <v>43609</v>
+      </c>
+      <c r="E9" s="7"/>
       <c r="F9" s="6" t="s">
         <v>22</v>
       </c>
@@ -1472,8 +1552,13 @@
       <c r="I9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="J9" s="8"/>
-      <c r="L9" s="7"/>
+      <c r="J9" s="3"/>
+      <c r="K9" t="s">
+        <v>37</v>
+      </c>
+      <c r="L9" s="2">
+        <v>43608</v>
+      </c>
       <c r="M9" s="6">
         <v>1</v>
       </c>
@@ -1483,9 +1568,12 @@
       <c r="O9">
         <v>8</v>
       </c>
-      <c r="Q9" s="5" t="str">
-        <f t="shared" ref="Q9" si="1">CONCATENATE(O9,"_",P9)</f>
-        <v>8_</v>
+      <c r="P9">
+        <v>19052301</v>
+      </c>
+      <c r="Q9" t="str">
+        <f t="shared" si="0"/>
+        <v>8_19052301</v>
       </c>
     </row>
     <row r="10" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1493,15 +1581,15 @@
         <v>15</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D10" s="2">
-        <v>43605</v>
-      </c>
-      <c r="E10" s="8"/>
+        <v>43609</v>
+      </c>
+      <c r="E10" s="7"/>
       <c r="F10" s="5" t="s">
         <v>22</v>
       </c>
@@ -1514,8 +1602,13 @@
       <c r="I10" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="J10" s="8"/>
-      <c r="L10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" t="s">
+        <v>37</v>
+      </c>
+      <c r="L10" s="2">
+        <v>43608</v>
+      </c>
       <c r="M10" s="6">
         <v>2</v>
       </c>
@@ -1525,9 +1618,12 @@
       <c r="O10">
         <v>9</v>
       </c>
-      <c r="Q10" s="5" t="str">
-        <f>CONCATENATE(O10,"_",P10)</f>
-        <v>9_</v>
+      <c r="P10">
+        <v>19052301</v>
+      </c>
+      <c r="Q10" t="str">
+        <f t="shared" si="0"/>
+        <v>9_19052301</v>
       </c>
     </row>
     <row r="11" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1535,15 +1631,15 @@
         <v>15</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="2">
-        <v>43605</v>
-      </c>
-      <c r="E11" s="8"/>
+        <v>43609</v>
+      </c>
+      <c r="E11" s="7"/>
       <c r="F11" s="5" t="s">
         <v>18</v>
       </c>
@@ -1556,8 +1652,13 @@
       <c r="I11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="8"/>
-      <c r="L11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" t="s">
+        <v>37</v>
+      </c>
+      <c r="L11" s="2">
+        <v>43608</v>
+      </c>
       <c r="M11" s="6">
         <v>1</v>
       </c>
@@ -1567,9 +1668,12 @@
       <c r="O11">
         <v>10</v>
       </c>
-      <c r="Q11" s="5" t="str">
-        <f>CONCATENATE(O11,"_",P11)</f>
-        <v>10_</v>
+      <c r="P11">
+        <v>19052301</v>
+      </c>
+      <c r="Q11" t="str">
+        <f t="shared" si="0"/>
+        <v>10_19052301</v>
       </c>
     </row>
     <row r="12" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1577,15 +1681,15 @@
         <v>15</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="2">
-        <v>43605</v>
-      </c>
-      <c r="E12" s="8"/>
+        <v>43609</v>
+      </c>
+      <c r="E12" s="7"/>
       <c r="F12" s="5" t="s">
         <v>18</v>
       </c>
@@ -1598,8 +1702,13 @@
       <c r="I12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J12" s="8"/>
-      <c r="L12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" t="s">
+        <v>37</v>
+      </c>
+      <c r="L12" s="2">
+        <v>43608</v>
+      </c>
       <c r="M12" s="6">
         <v>2</v>
       </c>
@@ -1609,9 +1718,12 @@
       <c r="O12">
         <v>11</v>
       </c>
-      <c r="Q12" s="5" t="str">
-        <f>CONCATENATE(O12,"_",P12)</f>
-        <v>11_</v>
+      <c r="P12">
+        <v>19052301</v>
+      </c>
+      <c r="Q12" t="str">
+        <f t="shared" si="0"/>
+        <v>11_19052301</v>
       </c>
     </row>
     <row r="13" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1619,15 +1731,15 @@
         <v>15</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="2">
-        <v>43605</v>
-      </c>
-      <c r="E13" s="8"/>
+        <v>43609</v>
+      </c>
+      <c r="E13" s="7"/>
       <c r="F13" s="5" t="s">
         <v>18</v>
       </c>
@@ -1638,12 +1750,17 @@
         <v>0.25</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J13" s="8"/>
-      <c r="L13" s="7"/>
+        <v>23</v>
+      </c>
+      <c r="J13" s="7"/>
+      <c r="K13" t="s">
+        <v>37</v>
+      </c>
+      <c r="L13" s="2">
+        <v>43608</v>
+      </c>
       <c r="M13" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N13" s="5" t="s">
         <v>25</v>
@@ -1651,9 +1768,12 @@
       <c r="O13">
         <v>12</v>
       </c>
-      <c r="Q13" s="5" t="str">
-        <f>CONCATENATE(O13,"_",P13)</f>
-        <v>12_</v>
+      <c r="P13">
+        <v>19052301</v>
+      </c>
+      <c r="Q13" t="str">
+        <f t="shared" si="0"/>
+        <v>12_19052301</v>
       </c>
     </row>
     <row r="14" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1661,15 +1781,15 @@
         <v>15</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D14" s="2">
-        <v>43605</v>
-      </c>
-      <c r="E14" s="8"/>
+        <v>43609</v>
+      </c>
+      <c r="E14" s="7"/>
       <c r="F14" s="5" t="s">
         <v>18</v>
       </c>
@@ -1682,10 +1802,15 @@
       <c r="I14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="8"/>
-      <c r="L14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" t="s">
+        <v>37</v>
+      </c>
+      <c r="L14" s="2">
+        <v>43608</v>
+      </c>
       <c r="M14" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N14" s="5" t="s">
         <v>25</v>
@@ -1693,9 +1818,12 @@
       <c r="O14">
         <v>13</v>
       </c>
-      <c r="Q14" s="5" t="str">
-        <f>CONCATENATE(O14,"_",P14)</f>
-        <v>13_</v>
+      <c r="P14">
+        <v>19052301</v>
+      </c>
+      <c r="Q14" t="str">
+        <f t="shared" si="0"/>
+        <v>13_19052301</v>
       </c>
     </row>
     <row r="15" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1703,31 +1831,36 @@
         <v>15</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="2">
-        <v>43605</v>
-      </c>
-      <c r="E15" s="8"/>
+        <v>43609</v>
+      </c>
+      <c r="E15" s="7"/>
       <c r="F15" s="5" t="s">
         <v>18</v>
       </c>
       <c r="G15" s="5">
-        <v>8</v>
+        <v>0.25</v>
       </c>
       <c r="H15" s="5">
-        <v>8</v>
+        <v>0.25</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J15" s="8"/>
-      <c r="L15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" t="s">
+        <v>37</v>
+      </c>
+      <c r="L15" s="2">
+        <v>43608</v>
+      </c>
       <c r="M15" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N15" s="5" t="s">
         <v>25</v>
@@ -1735,9 +1868,12 @@
       <c r="O15">
         <v>14</v>
       </c>
-      <c r="Q15" s="5" t="str">
-        <f>CONCATENATE(O15,"_",P15)</f>
-        <v>14_</v>
+      <c r="P15">
+        <v>19052301</v>
+      </c>
+      <c r="Q15" t="str">
+        <f t="shared" si="0"/>
+        <v>14_19052301</v>
       </c>
     </row>
     <row r="16" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1745,15 +1881,15 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D16" s="2">
-        <v>43605</v>
-      </c>
-      <c r="E16" s="8"/>
+        <v>43609</v>
+      </c>
+      <c r="E16" s="7"/>
       <c r="F16" s="5" t="s">
         <v>18</v>
       </c>
@@ -1766,10 +1902,15 @@
       <c r="I16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="8"/>
-      <c r="L16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" t="s">
+        <v>37</v>
+      </c>
+      <c r="L16" s="2">
+        <v>43608</v>
+      </c>
       <c r="M16" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N16" s="5" t="s">
         <v>25</v>
@@ -1777,9 +1918,12 @@
       <c r="O16">
         <v>15</v>
       </c>
-      <c r="Q16" s="5" t="str">
-        <f>CONCATENATE(O16,"_",P16)</f>
-        <v>15_</v>
+      <c r="P16">
+        <v>19052301</v>
+      </c>
+      <c r="Q16" t="str">
+        <f t="shared" si="0"/>
+        <v>15_19052301</v>
       </c>
     </row>
     <row r="17" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1787,31 +1931,36 @@
         <v>15</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>28</v>
+        <v>38</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="D17" s="2">
-        <v>43605</v>
-      </c>
-      <c r="E17" s="8"/>
+        <v>43609</v>
+      </c>
+      <c r="E17" s="7"/>
       <c r="F17" s="5" t="s">
         <v>18</v>
       </c>
       <c r="G17" s="5">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H17" s="5">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J17" s="8"/>
-      <c r="L17" s="7"/>
+        <v>19</v>
+      </c>
+      <c r="J17" s="7"/>
+      <c r="K17" t="s">
+        <v>37</v>
+      </c>
+      <c r="L17" s="2">
+        <v>43608</v>
+      </c>
       <c r="M17" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N17" s="5" t="s">
         <v>25</v>
@@ -1819,9 +1968,12 @@
       <c r="O17">
         <v>16</v>
       </c>
-      <c r="Q17" s="5" t="str">
-        <f>CONCATENATE(O17,"_",P17)</f>
-        <v>16_</v>
+      <c r="P17">
+        <v>19052301</v>
+      </c>
+      <c r="Q17" t="str">
+        <f t="shared" si="0"/>
+        <v>16_19052301</v>
       </c>
     </row>
     <row r="18" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1829,15 +1981,15 @@
         <v>15</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D18" s="2">
-        <v>43605</v>
-      </c>
-      <c r="E18" s="8"/>
+        <v>43609</v>
+      </c>
+      <c r="E18" s="7"/>
       <c r="F18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1850,10 +2002,15 @@
       <c r="I18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="8"/>
-      <c r="L18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" t="s">
+        <v>37</v>
+      </c>
+      <c r="L18" s="2">
+        <v>43608</v>
+      </c>
       <c r="M18" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N18" s="5" t="s">
         <v>25</v>
@@ -1861,9 +2018,12 @@
       <c r="O18">
         <v>17</v>
       </c>
+      <c r="P18">
+        <v>19052301</v>
+      </c>
       <c r="Q18" s="5" t="str">
-        <f>CONCATENATE(O18,"_",P18)</f>
-        <v>17_</v>
+        <f t="shared" ref="Q18:Q52" si="1">CONCATENATE(O18,"_",P18)</f>
+        <v>17_19052301</v>
       </c>
     </row>
     <row r="19" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1871,15 +2031,15 @@
         <v>15</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D19" s="2">
-        <v>43605</v>
-      </c>
-      <c r="E19" s="8"/>
+        <v>43609</v>
+      </c>
+      <c r="E19" s="7"/>
       <c r="F19" s="5" t="s">
         <v>18</v>
       </c>
@@ -1890,12 +2050,17 @@
         <v>0</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J19" s="8"/>
-      <c r="L19" s="7"/>
+        <v>23</v>
+      </c>
+      <c r="J19" s="7"/>
+      <c r="K19" t="s">
+        <v>37</v>
+      </c>
+      <c r="L19" s="2">
+        <v>43608</v>
+      </c>
       <c r="M19" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N19" s="5" t="s">
         <v>25</v>
@@ -1903,9 +2068,12 @@
       <c r="O19">
         <v>18</v>
       </c>
+      <c r="P19">
+        <v>19052301</v>
+      </c>
       <c r="Q19" s="5" t="str">
-        <f>CONCATENATE(O19,"_",P19)</f>
-        <v>18_</v>
+        <f t="shared" si="1"/>
+        <v>18_19052301</v>
       </c>
     </row>
     <row r="20" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1913,15 +2081,15 @@
         <v>15</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D20" s="2">
-        <v>43605</v>
-      </c>
-      <c r="E20" s="8"/>
+        <v>43609</v>
+      </c>
+      <c r="E20" s="7"/>
       <c r="F20" s="5" t="s">
         <v>18</v>
       </c>
@@ -1934,10 +2102,15 @@
       <c r="I20" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J20" s="8"/>
-      <c r="L20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" t="s">
+        <v>37</v>
+      </c>
+      <c r="L20" s="2">
+        <v>43608</v>
+      </c>
       <c r="M20" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N20" s="5" t="s">
         <v>25</v>
@@ -1945,1058 +2118,1262 @@
       <c r="O20">
         <v>19</v>
       </c>
+      <c r="P20">
+        <v>19052301</v>
+      </c>
       <c r="Q20" s="5" t="str">
-        <f>CONCATENATE(O20,"_",P20)</f>
-        <v>19_</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="9">
+        <f t="shared" si="1"/>
+        <v>19_19052301</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21">
         <v>15</v>
       </c>
-      <c r="B21" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>24</v>
+      <c r="B21" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="D21" s="2">
-        <v>43605</v>
-      </c>
-      <c r="E21" s="12"/>
-      <c r="F21" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I21" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="J21" s="12"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="10">
-        <v>1</v>
-      </c>
-      <c r="N21" s="9" t="s">
+        <v>43609</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" s="5">
+        <v>0</v>
+      </c>
+      <c r="H21" s="5">
+        <v>0</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21" s="7"/>
+      <c r="K21" t="s">
+        <v>37</v>
+      </c>
+      <c r="L21" s="2">
+        <v>43608</v>
+      </c>
+      <c r="M21" s="6">
+        <v>2</v>
+      </c>
+      <c r="N21" s="5" t="s">
         <v>25</v>
       </c>
       <c r="O21">
         <v>20</v>
       </c>
-      <c r="Q21" s="9" t="str">
-        <f>CONCATENATE(O21,"_",P21)</f>
-        <v>20_</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="9">
-        <v>15</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>30</v>
+      <c r="P21">
+        <v>19052301</v>
+      </c>
+      <c r="Q21" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>20_19052301</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="8">
+        <v>33</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="2">
-        <v>43605</v>
-      </c>
-      <c r="E22" s="12"/>
+      <c r="D22" s="10">
+        <v>43608</v>
+      </c>
+      <c r="E22" s="11"/>
       <c r="F22" s="9" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>16</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="J22" s="12"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="10">
-        <v>2</v>
-      </c>
-      <c r="N22" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="J22" s="11"/>
+      <c r="K22" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L22" s="10">
+        <v>43608</v>
+      </c>
+      <c r="M22" s="9">
+        <v>1</v>
+      </c>
+      <c r="N22" s="8" t="s">
         <v>25</v>
       </c>
       <c r="O22">
         <v>21</v>
       </c>
-      <c r="Q22" s="9" t="str">
-        <f>CONCATENATE(O22,"_",P22)</f>
-        <v>21_</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="9">
-        <v>15</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="9" t="s">
+      <c r="P22" s="8">
+        <v>19052301</v>
+      </c>
+      <c r="Q22" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>21_19052301</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="8">
+        <v>33</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="2">
-        <v>43605</v>
-      </c>
-      <c r="E23" s="12"/>
+      <c r="D23" s="10">
+        <v>43608</v>
+      </c>
+      <c r="E23" s="11"/>
       <c r="F23" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G23" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="H23" s="9">
-        <v>0.25</v>
+        <v>36</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J23" s="12"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="10">
-        <v>1</v>
-      </c>
-      <c r="N23" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="J23" s="11"/>
+      <c r="K23" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L23" s="10">
+        <v>43608</v>
+      </c>
+      <c r="M23" s="9">
+        <v>2</v>
+      </c>
+      <c r="N23" s="8" t="s">
         <v>25</v>
       </c>
       <c r="O23">
         <v>22</v>
       </c>
-      <c r="Q23" s="9" t="str">
-        <f>CONCATENATE(O23,"_",P23)</f>
-        <v>22_</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="9">
-        <v>15</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="9" t="s">
+      <c r="P23" s="8">
+        <v>19052301</v>
+      </c>
+      <c r="Q23" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>22_19052301</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="8">
+        <v>33</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="2">
-        <v>43605</v>
-      </c>
-      <c r="E24" s="12"/>
+      <c r="D24" s="10">
+        <v>43608</v>
+      </c>
+      <c r="E24" s="11"/>
       <c r="F24" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G24" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="H24" s="9">
-        <v>0.25</v>
+        <v>36</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J24" s="12"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="10">
-        <v>2</v>
-      </c>
-      <c r="N24" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="J24" s="11"/>
+      <c r="K24" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L24" s="10">
+        <v>43608</v>
+      </c>
+      <c r="M24" s="9">
+        <v>1</v>
+      </c>
+      <c r="N24" s="8" t="s">
         <v>25</v>
       </c>
       <c r="O24">
         <v>23</v>
       </c>
-      <c r="Q24" s="9" t="str">
-        <f>CONCATENATE(O24,"_",P24)</f>
-        <v>23_</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="9">
-        <v>15</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>30</v>
+      <c r="P24" s="8">
+        <v>19052301</v>
+      </c>
+      <c r="Q24" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>23_19052301</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="8">
+        <v>33</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="2">
-        <v>43605</v>
-      </c>
-      <c r="E25" s="12"/>
+      <c r="D25" s="10">
+        <v>43608</v>
+      </c>
+      <c r="E25" s="11"/>
       <c r="F25" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G25" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="H25" s="9">
-        <v>0.25</v>
+        <v>36</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="J25" s="12"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="10">
-        <v>1</v>
-      </c>
-      <c r="N25" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="J25" s="11"/>
+      <c r="K25" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L25" s="10">
+        <v>43608</v>
+      </c>
+      <c r="M25" s="9">
+        <v>2</v>
+      </c>
+      <c r="N25" s="8" t="s">
         <v>25</v>
       </c>
       <c r="O25">
         <v>24</v>
       </c>
-      <c r="Q25" s="9" t="str">
-        <f>CONCATENATE(O25,"_",P25)</f>
-        <v>24_</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="9">
-        <v>15</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="9" t="s">
+      <c r="P25" s="8">
+        <v>19052301</v>
+      </c>
+      <c r="Q25" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>24_19052301</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="8">
+        <v>33</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="2">
-        <v>43605</v>
-      </c>
-      <c r="E26" s="12"/>
+      <c r="D26" s="10">
+        <v>43608</v>
+      </c>
+      <c r="E26" s="11"/>
       <c r="F26" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G26" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="H26" s="9">
-        <v>0.25</v>
+        <v>36</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="J26" s="12"/>
-      <c r="L26" s="11"/>
-      <c r="M26" s="10">
+        <v>35</v>
+      </c>
+      <c r="J26" s="11"/>
+      <c r="K26" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L26" s="10">
+        <v>43608</v>
+      </c>
+      <c r="M26" s="9">
+        <v>1</v>
+      </c>
+      <c r="N26" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O26">
+        <v>25</v>
+      </c>
+      <c r="P26" s="8">
+        <v>19052301</v>
+      </c>
+      <c r="Q26" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>25_19052301</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="8">
+        <v>33</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="10">
+        <v>43608</v>
+      </c>
+      <c r="E27" s="11"/>
+      <c r="F27" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="J27" s="11"/>
+      <c r="K27" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L27" s="10">
+        <v>43608</v>
+      </c>
+      <c r="M27" s="9">
         <v>2</v>
       </c>
-      <c r="N26" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="O26">
-        <v>25</v>
-      </c>
-      <c r="Q26" s="9" t="str">
-        <f>CONCATENATE(O26,"_",P26)</f>
-        <v>25_</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="9">
-        <v>15</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27" s="2">
-        <v>43605</v>
-      </c>
-      <c r="E27" s="12"/>
-      <c r="F27" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G27" s="9">
-        <v>8</v>
-      </c>
-      <c r="H27" s="9">
-        <v>8</v>
-      </c>
-      <c r="I27" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="J27" s="12"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="10">
-        <v>1</v>
-      </c>
-      <c r="N27" s="9" t="s">
+      <c r="N27" s="8" t="s">
         <v>25</v>
       </c>
       <c r="O27">
         <v>26</v>
       </c>
-      <c r="Q27" s="9" t="str">
-        <f>CONCATENATE(O27,"_",P27)</f>
-        <v>26_</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="9">
-        <v>15</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>30</v>
+      <c r="P27" s="8">
+        <v>19052301</v>
+      </c>
+      <c r="Q27" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>26_19052301</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="8">
+        <v>33</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="2">
-        <v>43605</v>
-      </c>
-      <c r="E28" s="12"/>
+      <c r="D28" s="10">
+        <v>43608</v>
+      </c>
+      <c r="E28" s="11"/>
       <c r="F28" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G28" s="9">
-        <v>8</v>
-      </c>
-      <c r="H28" s="9">
-        <v>8</v>
+        <v>36</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="J28" s="12"/>
-      <c r="L28" s="11"/>
-      <c r="M28" s="10">
-        <v>2</v>
-      </c>
-      <c r="N28" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="J28" s="11"/>
+      <c r="K28" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L28" s="10">
+        <v>43608</v>
+      </c>
+      <c r="M28" s="9">
+        <v>1</v>
+      </c>
+      <c r="N28" s="8" t="s">
         <v>25</v>
       </c>
       <c r="O28">
         <v>27</v>
       </c>
-      <c r="Q28" s="9" t="str">
-        <f>CONCATENATE(O28,"_",P28)</f>
-        <v>27_</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="9">
-        <v>15</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D29" s="2">
-        <v>43605</v>
-      </c>
-      <c r="E29" s="12"/>
+      <c r="P28" s="8">
+        <v>19052301</v>
+      </c>
+      <c r="Q28" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>27_19052301</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="8">
+        <v>33</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" s="10">
+        <v>43608</v>
+      </c>
+      <c r="E29" s="11"/>
       <c r="F29" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G29" s="9">
-        <v>0</v>
-      </c>
-      <c r="H29" s="9">
-        <v>0</v>
+        <v>36</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J29" s="12"/>
-      <c r="L29" s="11"/>
-      <c r="M29" s="10">
-        <v>1</v>
-      </c>
-      <c r="N29" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="J29" s="11"/>
+      <c r="K29" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L29" s="10">
+        <v>43608</v>
+      </c>
+      <c r="M29" s="9">
+        <v>2</v>
+      </c>
+      <c r="N29" s="8" t="s">
         <v>25</v>
       </c>
       <c r="O29">
         <v>28</v>
       </c>
-      <c r="Q29" s="9" t="str">
-        <f>CONCATENATE(O29,"_",P29)</f>
-        <v>28_</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="9">
-        <v>15</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D30" s="2">
-        <v>43605</v>
-      </c>
-      <c r="E30" s="12"/>
+      <c r="P29" s="8">
+        <v>19052301</v>
+      </c>
+      <c r="Q29" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>28_19052301</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="8">
+        <v>33</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="10">
+        <v>43608</v>
+      </c>
+      <c r="E30" s="11"/>
       <c r="F30" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G30" s="9">
-        <v>0</v>
-      </c>
-      <c r="H30" s="9">
-        <v>0</v>
+        <v>36</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J30" s="12"/>
-      <c r="L30" s="11"/>
-      <c r="M30" s="10">
-        <v>2</v>
-      </c>
-      <c r="N30" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="J30" s="11"/>
+      <c r="K30" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L30" s="10">
+        <v>43608</v>
+      </c>
+      <c r="M30" s="9">
+        <v>1</v>
+      </c>
+      <c r="N30" s="8" t="s">
         <v>25</v>
       </c>
       <c r="O30">
         <v>29</v>
       </c>
-      <c r="Q30" s="9" t="str">
-        <f>CONCATENATE(O30,"_",P30)</f>
-        <v>29_</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="9">
-        <v>15</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D31" s="2">
-        <v>43605</v>
-      </c>
-      <c r="E31" s="12"/>
+      <c r="P30" s="8">
+        <v>19052301</v>
+      </c>
+      <c r="Q30" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>29_19052301</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="8">
+        <v>33</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="10">
+        <v>43608</v>
+      </c>
+      <c r="E31" s="11"/>
       <c r="F31" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G31" s="9">
-        <v>0</v>
-      </c>
-      <c r="H31" s="9">
-        <v>0</v>
+        <v>36</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="J31" s="12"/>
-      <c r="L31" s="11"/>
-      <c r="M31" s="10">
-        <v>1</v>
-      </c>
-      <c r="N31" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="J31" s="11"/>
+      <c r="K31" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L31" s="10">
+        <v>43608</v>
+      </c>
+      <c r="M31" s="9">
+        <v>2</v>
+      </c>
+      <c r="N31" s="8" t="s">
         <v>25</v>
       </c>
       <c r="O31">
         <v>30</v>
       </c>
-      <c r="Q31" s="9" t="str">
-        <f>CONCATENATE(O31,"_",P31)</f>
-        <v>30_</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="9">
-        <v>15</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D32" s="2">
-        <v>43605</v>
-      </c>
-      <c r="E32" s="12"/>
+      <c r="P31" s="8">
+        <v>19052301</v>
+      </c>
+      <c r="Q31" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>30_19052301</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="8">
+        <v>33</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="10">
+        <v>43608</v>
+      </c>
+      <c r="E32" s="11"/>
       <c r="F32" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G32" s="9">
-        <v>0</v>
-      </c>
-      <c r="H32" s="9">
-        <v>0</v>
+        <v>36</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="J32" s="12"/>
-      <c r="L32" s="11"/>
-      <c r="M32" s="10">
-        <v>2</v>
-      </c>
-      <c r="N32" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="J32" s="11"/>
+      <c r="K32" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L32" s="10">
+        <v>43608</v>
+      </c>
+      <c r="M32" s="9">
+        <v>1</v>
+      </c>
+      <c r="N32" s="8" t="s">
         <v>25</v>
       </c>
       <c r="O32">
         <v>31</v>
       </c>
-      <c r="Q32" s="9" t="str">
-        <f>CONCATENATE(O32,"_",P32)</f>
-        <v>31_</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="13">
-        <v>15</v>
-      </c>
-      <c r="B33" s="14" t="s">
+      <c r="P32" s="8">
+        <v>19052301</v>
+      </c>
+      <c r="Q32" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>31_19052301</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="8">
+        <v>33</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="10">
+        <v>43608</v>
+      </c>
+      <c r="E33" s="11"/>
+      <c r="F33" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D33" s="15">
-        <v>43600</v>
-      </c>
-      <c r="E33" s="16"/>
-      <c r="F33" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="G33" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H33" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I33" s="14" t="s">
+      <c r="G33" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="J33" s="16"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="14">
+      <c r="H33" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="J33" s="11"/>
+      <c r="K33" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L33" s="10">
+        <v>43608</v>
+      </c>
+      <c r="M33" s="9">
         <v>1</v>
       </c>
-      <c r="N33" s="13" t="s">
+      <c r="N33" s="8" t="s">
         <v>25</v>
       </c>
       <c r="O33">
         <v>32</v>
       </c>
-      <c r="Q33" s="13" t="str">
-        <f>CONCATENATE(O33,"_",P33)</f>
-        <v>32_</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="13">
-        <v>15</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>36</v>
+      <c r="P33" s="8">
+        <v>19052301</v>
+      </c>
+      <c r="Q33" s="8" t="str">
+        <f t="shared" ref="Q33:Q44" si="2">CONCATENATE(O33,"_",P33)</f>
+        <v>32_19052301</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="12">
+        <v>33</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="15">
-        <v>43600</v>
-      </c>
-      <c r="E34" s="16"/>
-      <c r="F34" s="14" t="s">
-        <v>43</v>
+      <c r="D34" s="14">
+        <v>43608</v>
+      </c>
+      <c r="E34" s="15"/>
+      <c r="F34" s="13" t="s">
+        <v>36</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="H34" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I34" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="J34" s="16"/>
-      <c r="L34" s="15"/>
-      <c r="M34" s="14">
-        <v>2</v>
-      </c>
-      <c r="N34" s="13" t="s">
+      <c r="I34" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="J34" s="15"/>
+      <c r="K34" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="L34" s="14">
+        <v>43608</v>
+      </c>
+      <c r="M34" s="13">
+        <v>1</v>
+      </c>
+      <c r="N34" s="12" t="s">
         <v>25</v>
       </c>
       <c r="O34">
         <v>33</v>
       </c>
-      <c r="Q34" s="13" t="str">
-        <f>CONCATENATE(O34,"_",P34)</f>
-        <v>33_</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="13">
-        <v>15</v>
-      </c>
-      <c r="B35" s="14" t="s">
+      <c r="P34" s="12">
+        <v>19052301</v>
+      </c>
+      <c r="Q34" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>33_19052301</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="12">
+        <v>33</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" s="14">
+        <v>43608</v>
+      </c>
+      <c r="E35" s="15"/>
+      <c r="F35" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D35" s="15">
-        <v>43600</v>
-      </c>
-      <c r="E35" s="16"/>
-      <c r="F35" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="G35" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H35" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I35" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="J35" s="16"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="14">
-        <v>1</v>
-      </c>
-      <c r="N35" s="13" t="s">
+      <c r="G35" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="H35" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I35" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="J35" s="15"/>
+      <c r="K35" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="L35" s="14">
+        <v>43608</v>
+      </c>
+      <c r="M35" s="13">
+        <v>2</v>
+      </c>
+      <c r="N35" s="12" t="s">
         <v>25</v>
       </c>
       <c r="O35">
         <v>34</v>
       </c>
-      <c r="Q35" s="13" t="str">
-        <f>CONCATENATE(O35,"_",P35)</f>
-        <v>34_</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="13">
-        <v>15</v>
-      </c>
-      <c r="B36" s="14" t="s">
+      <c r="P35" s="12">
+        <v>19052301</v>
+      </c>
+      <c r="Q35" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>34_19052301</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="12">
+        <v>33</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" s="14">
+        <v>43608</v>
+      </c>
+      <c r="E36" s="15"/>
+      <c r="F36" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D36" s="15">
-        <v>43600</v>
-      </c>
-      <c r="E36" s="16"/>
-      <c r="F36" s="14" t="s">
-        <v>43</v>
-      </c>
       <c r="G36" s="13" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="H36" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I36" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="J36" s="16"/>
-      <c r="L36" s="15"/>
-      <c r="M36" s="14">
-        <v>2</v>
-      </c>
-      <c r="N36" s="13" t="s">
+      <c r="I36" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="J36" s="15"/>
+      <c r="K36" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="L36" s="14">
+        <v>43608</v>
+      </c>
+      <c r="M36" s="13">
+        <v>1</v>
+      </c>
+      <c r="N36" s="12" t="s">
         <v>25</v>
       </c>
       <c r="O36">
         <v>35</v>
       </c>
-      <c r="Q36" s="13" t="str">
-        <f>CONCATENATE(O36,"_",P36)</f>
-        <v>35_</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="13">
-        <v>15</v>
-      </c>
-      <c r="B37" s="14" t="s">
+      <c r="P36" s="12">
+        <v>19052301</v>
+      </c>
+      <c r="Q36" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>35_19052301</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="12">
+        <v>33</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" s="14">
+        <v>43608</v>
+      </c>
+      <c r="E37" s="15"/>
+      <c r="F37" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D37" s="15">
-        <v>43600</v>
-      </c>
-      <c r="E37" s="16"/>
-      <c r="F37" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="G37" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H37" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I37" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="J37" s="16"/>
-      <c r="L37" s="15"/>
-      <c r="M37" s="14">
-        <v>1</v>
-      </c>
-      <c r="N37" s="13" t="s">
+      <c r="G37" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H37" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I37" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="J37" s="15"/>
+      <c r="K37" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="L37" s="14">
+        <v>43608</v>
+      </c>
+      <c r="M37" s="13">
+        <v>2</v>
+      </c>
+      <c r="N37" s="12" t="s">
         <v>25</v>
       </c>
       <c r="O37">
         <v>36</v>
       </c>
-      <c r="Q37" s="13" t="str">
-        <f>CONCATENATE(O37,"_",P37)</f>
-        <v>36_</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="13">
-        <v>15</v>
-      </c>
-      <c r="B38" s="14" t="s">
+      <c r="P37" s="12">
+        <v>19052301</v>
+      </c>
+      <c r="Q37" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>36_19052301</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="12">
+        <v>33</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" s="14">
+        <v>43608</v>
+      </c>
+      <c r="E38" s="15"/>
+      <c r="F38" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="G38" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D38" s="15">
-        <v>43600</v>
-      </c>
-      <c r="E38" s="16"/>
-      <c r="F38" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="G38" s="13" t="s">
-        <v>16</v>
-      </c>
       <c r="H38" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I38" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="J38" s="16"/>
-      <c r="L38" s="15"/>
-      <c r="M38" s="14">
+      <c r="I38" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="J38" s="15"/>
+      <c r="K38" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="L38" s="14">
+        <v>43608</v>
+      </c>
+      <c r="M38" s="13">
+        <v>1</v>
+      </c>
+      <c r="N38" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="O38">
+        <v>37</v>
+      </c>
+      <c r="P38" s="12">
+        <v>19052301</v>
+      </c>
+      <c r="Q38" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>37_19052301</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="12">
+        <v>33</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" s="14">
+        <v>43608</v>
+      </c>
+      <c r="E39" s="15"/>
+      <c r="F39" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H39" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I39" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="J39" s="15"/>
+      <c r="K39" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="L39" s="14">
+        <v>43608</v>
+      </c>
+      <c r="M39" s="13">
         <v>2</v>
       </c>
-      <c r="N38" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="O38">
-        <v>37</v>
-      </c>
-      <c r="Q38" s="13" t="str">
-        <f>CONCATENATE(O38,"_",P38)</f>
-        <v>37_</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="13">
-        <v>15</v>
-      </c>
-      <c r="B39" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D39" s="15">
-        <v>43600</v>
-      </c>
-      <c r="E39" s="16"/>
-      <c r="F39" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="G39" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H39" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I39" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="J39" s="16"/>
-      <c r="L39" s="15"/>
-      <c r="M39" s="14">
-        <v>1</v>
-      </c>
-      <c r="N39" s="13" t="s">
+      <c r="N39" s="12" t="s">
         <v>25</v>
       </c>
       <c r="O39">
         <v>38</v>
       </c>
-      <c r="Q39" s="13" t="str">
-        <f>CONCATENATE(O39,"_",P39)</f>
-        <v>38_</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="13">
-        <v>15</v>
-      </c>
-      <c r="B40" s="14" t="s">
-        <v>37</v>
+      <c r="P39" s="12">
+        <v>19052301</v>
+      </c>
+      <c r="Q39" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>38_19052301</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="12">
+        <v>33</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="C40" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D40" s="15">
-        <v>43600</v>
-      </c>
-      <c r="E40" s="16"/>
-      <c r="F40" s="14" t="s">
-        <v>43</v>
+      <c r="D40" s="14">
+        <v>43608</v>
+      </c>
+      <c r="E40" s="15"/>
+      <c r="F40" s="13" t="s">
+        <v>36</v>
       </c>
       <c r="G40" s="13" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="H40" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I40" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="J40" s="16"/>
-      <c r="L40" s="15"/>
-      <c r="M40" s="14">
-        <v>2</v>
-      </c>
-      <c r="N40" s="13" t="s">
+      <c r="I40" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="J40" s="15"/>
+      <c r="K40" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="L40" s="14">
+        <v>43608</v>
+      </c>
+      <c r="M40" s="13">
+        <v>1</v>
+      </c>
+      <c r="N40" s="12" t="s">
         <v>25</v>
       </c>
       <c r="O40">
         <v>39</v>
       </c>
-      <c r="Q40" s="13" t="str">
-        <f>CONCATENATE(O40,"_",P40)</f>
-        <v>39_</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="13">
-        <v>15</v>
-      </c>
-      <c r="B41" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C41" s="14" t="s">
+      <c r="P40" s="12">
+        <v>19052301</v>
+      </c>
+      <c r="Q40" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>39_19052301</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="12">
+        <v>33</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="15">
-        <v>43600</v>
-      </c>
-      <c r="E41" s="16"/>
-      <c r="F41" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="G41" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H41" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I41" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="J41" s="16"/>
-      <c r="L41" s="15"/>
-      <c r="M41" s="14">
-        <v>1</v>
-      </c>
-      <c r="N41" s="13" t="s">
+      <c r="D41" s="14">
+        <v>43608</v>
+      </c>
+      <c r="E41" s="15"/>
+      <c r="F41" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G41" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H41" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I41" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="J41" s="15"/>
+      <c r="K41" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="L41" s="14">
+        <v>43608</v>
+      </c>
+      <c r="M41" s="13">
+        <v>2</v>
+      </c>
+      <c r="N41" s="12" t="s">
         <v>25</v>
       </c>
       <c r="O41">
         <v>40</v>
       </c>
-      <c r="Q41" s="13" t="str">
-        <f>CONCATENATE(O41,"_",P41)</f>
-        <v>40_</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="13">
-        <v>15</v>
-      </c>
-      <c r="B42" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C42" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D42" s="15">
-        <v>43600</v>
-      </c>
-      <c r="E42" s="16"/>
-      <c r="F42" s="14" t="s">
-        <v>43</v>
+      <c r="P41" s="12">
+        <v>19052301</v>
+      </c>
+      <c r="Q41" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>40_19052301</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="12">
+        <v>33</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D42" s="14">
+        <v>43608</v>
+      </c>
+      <c r="E42" s="15"/>
+      <c r="F42" s="13" t="s">
+        <v>36</v>
       </c>
       <c r="G42" s="13" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="H42" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I42" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="J42" s="16"/>
-      <c r="L42" s="15"/>
-      <c r="M42" s="14">
-        <v>2</v>
-      </c>
-      <c r="N42" s="13" t="s">
+      <c r="I42" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="J42" s="15"/>
+      <c r="K42" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="L42" s="14">
+        <v>43608</v>
+      </c>
+      <c r="M42" s="13">
+        <v>1</v>
+      </c>
+      <c r="N42" s="12" t="s">
         <v>25</v>
       </c>
       <c r="O42">
         <v>41</v>
       </c>
-      <c r="Q42" s="13" t="str">
-        <f>CONCATENATE(O42,"_",P42)</f>
-        <v>41_</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="13">
-        <v>15</v>
-      </c>
-      <c r="B43" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C43" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D43" s="15">
-        <v>43600</v>
-      </c>
-      <c r="E43" s="16"/>
-      <c r="F43" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="G43" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H43" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I43" s="14" t="s">
+      <c r="P42" s="12">
+        <v>19052301</v>
+      </c>
+      <c r="Q42" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>41_19052301</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="12">
+        <v>33</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" s="14">
+        <v>43608</v>
+      </c>
+      <c r="E43" s="15"/>
+      <c r="F43" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G43" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="J43" s="16"/>
-      <c r="L43" s="15"/>
-      <c r="M43" s="14">
-        <v>1</v>
-      </c>
-      <c r="N43" s="13" t="s">
+      <c r="H43" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I43" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="J43" s="15"/>
+      <c r="K43" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="L43" s="14">
+        <v>43608</v>
+      </c>
+      <c r="M43" s="13">
+        <v>2</v>
+      </c>
+      <c r="N43" s="12" t="s">
         <v>25</v>
       </c>
       <c r="O43">
         <v>42</v>
       </c>
-      <c r="Q43" s="13" t="str">
-        <f>CONCATENATE(O43,"_",P43)</f>
-        <v>42_</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>15</v>
-      </c>
-      <c r="B44" t="s">
-        <v>16</v>
-      </c>
-      <c r="C44" t="s">
-        <v>16</v>
-      </c>
-      <c r="D44" s="2">
-        <v>43605</v>
-      </c>
-      <c r="E44" s="3">
-        <v>43605</v>
-      </c>
-      <c r="F44" t="s">
-        <v>16</v>
-      </c>
-      <c r="G44" t="s">
-        <v>16</v>
-      </c>
-      <c r="H44" t="s">
-        <v>16</v>
-      </c>
-      <c r="I44" t="s">
-        <v>17</v>
-      </c>
-      <c r="L44" s="2"/>
-      <c r="M44" s="1">
-        <v>3</v>
-      </c>
-      <c r="N44" t="s">
+      <c r="P43" s="12">
+        <v>19052301</v>
+      </c>
+      <c r="Q43" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>42_19052301</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="12">
+        <v>33</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D44" s="14">
+        <v>43608</v>
+      </c>
+      <c r="E44" s="15"/>
+      <c r="F44" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H44" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I44" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="J44" s="15"/>
+      <c r="K44" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="L44" s="14">
+        <v>43608</v>
+      </c>
+      <c r="M44" s="13">
+        <v>1</v>
+      </c>
+      <c r="N44" s="12" t="s">
         <v>25</v>
       </c>
       <c r="O44">
         <v>43</v>
       </c>
-      <c r="Q44" t="str">
-        <f>CONCATENATE(O44,"_",P44)</f>
-        <v>43_</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>15</v>
-      </c>
-      <c r="B45" t="s">
-        <v>16</v>
-      </c>
-      <c r="C45" t="s">
-        <v>16</v>
-      </c>
-      <c r="D45" s="2">
-        <v>43605</v>
-      </c>
-      <c r="F45" t="s">
-        <v>16</v>
-      </c>
-      <c r="G45" t="s">
-        <v>16</v>
-      </c>
-      <c r="H45" t="s">
-        <v>16</v>
-      </c>
-      <c r="I45" t="s">
-        <v>31</v>
-      </c>
-      <c r="L45" s="2"/>
-      <c r="M45" s="1">
-        <v>2</v>
-      </c>
-      <c r="N45" t="s">
+      <c r="P44" s="12">
+        <v>19052301</v>
+      </c>
+      <c r="Q44" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v>43_19052301</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="12">
+        <v>33</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D45" s="14">
+        <v>43608</v>
+      </c>
+      <c r="E45" s="15"/>
+      <c r="F45" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H45" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I45" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="J45" s="15"/>
+      <c r="K45" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="L45" s="14">
+        <v>43608</v>
+      </c>
+      <c r="M45" s="13">
+        <v>1</v>
+      </c>
+      <c r="N45" s="12" t="s">
         <v>25</v>
       </c>
       <c r="O45">
         <v>44</v>
       </c>
-      <c r="Q45" t="str">
-        <f>CONCATENATE(O45,"_",P45)</f>
-        <v>44_</v>
+      <c r="P45" s="12">
+        <v>19052301</v>
+      </c>
+      <c r="Q45" s="12" t="str">
+        <f t="shared" ref="Q45" si="3">CONCATENATE(O45,"_",P45)</f>
+        <v>44_19052301</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.2">
@@ -3012,6 +3389,9 @@
       <c r="D46" s="2">
         <v>43605</v>
       </c>
+      <c r="E46" s="3">
+        <v>43608</v>
+      </c>
       <c r="F46" t="s">
         <v>16</v>
       </c>
@@ -3022,11 +3402,19 @@
         <v>16</v>
       </c>
       <c r="I46" t="s">
-        <v>32</v>
-      </c>
-      <c r="L46" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="J46" s="3">
+        <v>43608</v>
+      </c>
+      <c r="K46" t="s">
+        <v>37</v>
+      </c>
+      <c r="L46" s="2">
+        <v>43608</v>
+      </c>
       <c r="M46" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N46" t="s">
         <v>25</v>
@@ -3034,9 +3422,12 @@
       <c r="O46">
         <v>45</v>
       </c>
+      <c r="P46">
+        <v>19052301</v>
+      </c>
       <c r="Q46" t="str">
-        <f>CONCATENATE(O46,"_",P46)</f>
-        <v>45_</v>
+        <f t="shared" si="1"/>
+        <v>45_19052301</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
@@ -3052,6 +3443,9 @@
       <c r="D47" s="2">
         <v>43605</v>
       </c>
+      <c r="E47" s="3">
+        <v>43608</v>
+      </c>
       <c r="F47" t="s">
         <v>16</v>
       </c>
@@ -3062,9 +3456,17 @@
         <v>16</v>
       </c>
       <c r="I47" t="s">
-        <v>33</v>
-      </c>
-      <c r="L47" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="J47" s="3">
+        <v>43608</v>
+      </c>
+      <c r="K47" t="s">
+        <v>37</v>
+      </c>
+      <c r="L47" s="2">
+        <v>43608</v>
+      </c>
       <c r="M47" s="1">
         <v>2</v>
       </c>
@@ -3074,9 +3476,12 @@
       <c r="O47">
         <v>46</v>
       </c>
+      <c r="P47">
+        <v>19052301</v>
+      </c>
       <c r="Q47" t="str">
-        <f>CONCATENATE(O47,"_",P47)</f>
-        <v>46_</v>
+        <f t="shared" si="1"/>
+        <v>46_19052301</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
@@ -3092,6 +3497,9 @@
       <c r="D48" s="2">
         <v>43605</v>
       </c>
+      <c r="E48" s="3">
+        <v>43608</v>
+      </c>
       <c r="F48" t="s">
         <v>16</v>
       </c>
@@ -3102,9 +3510,17 @@
         <v>16</v>
       </c>
       <c r="I48" t="s">
-        <v>34</v>
-      </c>
-      <c r="L48" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="J48" s="3">
+        <v>43608</v>
+      </c>
+      <c r="K48" t="s">
+        <v>37</v>
+      </c>
+      <c r="L48" s="2">
+        <v>43608</v>
+      </c>
       <c r="M48" s="1">
         <v>2</v>
       </c>
@@ -3114,9 +3530,12 @@
       <c r="O48">
         <v>47</v>
       </c>
+      <c r="P48">
+        <v>19052301</v>
+      </c>
       <c r="Q48" t="str">
-        <f>CONCATENATE(O48,"_",P48)</f>
-        <v>47_</v>
+        <f t="shared" si="1"/>
+        <v>47_19052301</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
@@ -3132,6 +3551,9 @@
       <c r="D49" s="2">
         <v>43605</v>
       </c>
+      <c r="E49" s="3">
+        <v>43608</v>
+      </c>
       <c r="F49" t="s">
         <v>16</v>
       </c>
@@ -3142,9 +3564,17 @@
         <v>16</v>
       </c>
       <c r="I49" t="s">
-        <v>35</v>
-      </c>
-      <c r="L49" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="J49" s="3">
+        <v>43608</v>
+      </c>
+      <c r="K49" t="s">
+        <v>37</v>
+      </c>
+      <c r="L49" s="2">
+        <v>43608</v>
+      </c>
       <c r="M49" s="1">
         <v>2</v>
       </c>
@@ -3154,9 +3584,12 @@
       <c r="O49">
         <v>48</v>
       </c>
+      <c r="P49">
+        <v>19052301</v>
+      </c>
       <c r="Q49" t="str">
-        <f>CONCATENATE(O49,"_",P49)</f>
-        <v>48_</v>
+        <f t="shared" si="1"/>
+        <v>48_19052301</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.2">
@@ -3172,6 +3605,9 @@
       <c r="D50" s="2">
         <v>43605</v>
       </c>
+      <c r="E50" s="3">
+        <v>43608</v>
+      </c>
       <c r="F50" t="s">
         <v>16</v>
       </c>
@@ -3182,11 +3618,19 @@
         <v>16</v>
       </c>
       <c r="I50" t="s">
-        <v>17</v>
-      </c>
-      <c r="L50" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="J50" s="3">
+        <v>43608</v>
+      </c>
+      <c r="K50" t="s">
+        <v>37</v>
+      </c>
+      <c r="L50" s="2">
+        <v>43608</v>
+      </c>
       <c r="M50" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N50" t="s">
         <v>25</v>
@@ -3194,14 +3638,125 @@
       <c r="O50">
         <v>49</v>
       </c>
+      <c r="P50">
+        <v>19052301</v>
+      </c>
       <c r="Q50" t="str">
-        <f>CONCATENATE(O50,"_",P50)</f>
-        <v>49_</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="I57" t="s">
-        <v>41</v>
+        <f t="shared" si="1"/>
+        <v>49_19052301</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>15</v>
+      </c>
+      <c r="B51" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" t="s">
+        <v>16</v>
+      </c>
+      <c r="D51" s="2">
+        <v>43605</v>
+      </c>
+      <c r="E51" s="3">
+        <v>43608</v>
+      </c>
+      <c r="F51" t="s">
+        <v>16</v>
+      </c>
+      <c r="G51" t="s">
+        <v>16</v>
+      </c>
+      <c r="H51" t="s">
+        <v>16</v>
+      </c>
+      <c r="I51" t="s">
+        <v>31</v>
+      </c>
+      <c r="J51" s="3">
+        <v>43608</v>
+      </c>
+      <c r="K51" t="s">
+        <v>37</v>
+      </c>
+      <c r="L51" s="2">
+        <v>43608</v>
+      </c>
+      <c r="M51" s="1">
+        <v>2</v>
+      </c>
+      <c r="N51" t="s">
+        <v>25</v>
+      </c>
+      <c r="O51">
+        <v>50</v>
+      </c>
+      <c r="P51">
+        <v>19052301</v>
+      </c>
+      <c r="Q51" t="str">
+        <f t="shared" si="1"/>
+        <v>50_19052301</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>15</v>
+      </c>
+      <c r="B52" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" t="s">
+        <v>16</v>
+      </c>
+      <c r="D52" s="2">
+        <v>43605</v>
+      </c>
+      <c r="E52" s="3">
+        <v>43608</v>
+      </c>
+      <c r="F52" t="s">
+        <v>16</v>
+      </c>
+      <c r="G52" t="s">
+        <v>16</v>
+      </c>
+      <c r="H52" t="s">
+        <v>16</v>
+      </c>
+      <c r="I52" t="s">
+        <v>17</v>
+      </c>
+      <c r="J52" s="3">
+        <v>43608</v>
+      </c>
+      <c r="K52" t="s">
+        <v>37</v>
+      </c>
+      <c r="L52" s="2">
+        <v>43608</v>
+      </c>
+      <c r="M52" s="1">
+        <v>4</v>
+      </c>
+      <c r="N52" t="s">
+        <v>25</v>
+      </c>
+      <c r="O52">
+        <v>51</v>
+      </c>
+      <c r="P52">
+        <v>19052301</v>
+      </c>
+      <c r="Q52" t="str">
+        <f t="shared" si="1"/>
+        <v>51_19052301</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="I59" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>